<commit_message>
Atualizar do MER e do Backlog
</commit_message>
<xml_diff>
--- a/Apresentação Sprint 2/Backlog.xlsx
+++ b/Apresentação Sprint 2/Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinic\OneDrive\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizg\Downloads\BandTec\Pesquisa e Inovação - Profº Brandão\Projeto PI - Sprint2\Projeto-PI\Apresentação Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{747F5079-6732-4827-A462-4CACBD8EF8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F631B7-2739-4F58-A2F0-AC7A64EBB7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8385" yWindow="1725" windowWidth="7935" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>Nome</t>
   </si>
@@ -83,9 +83,6 @@
     <t>RF3</t>
   </si>
   <si>
-    <t>O software deve permitir que o usuario gere relatorios atraves dos dados obtidos.</t>
-  </si>
-  <si>
     <t>RF4</t>
   </si>
   <si>
@@ -110,24 +107,9 @@
     <t>O software deve permitir que o administrador efetue a manutenção (consulta, inclusão, exclusão e alteração) de dados.</t>
   </si>
   <si>
-    <t>Carlos Eduardo Batista</t>
-  </si>
-  <si>
     <t>Carlos Mascena</t>
   </si>
   <si>
-    <t>Gabriel Aguiar</t>
-  </si>
-  <si>
-    <t>Gabriel Dias</t>
-  </si>
-  <si>
-    <t>Lucas Félix</t>
-  </si>
-  <si>
-    <t>Winicius</t>
-  </si>
-  <si>
     <t>Desejável</t>
   </si>
   <si>
@@ -167,18 +149,9 @@
     <t>RF18</t>
   </si>
   <si>
-    <t>RF19</t>
-  </si>
-  <si>
-    <t>RF20</t>
-  </si>
-  <si>
     <t>O software deverá ter Wi-fi.</t>
   </si>
   <si>
-    <t>O software deverá ter um diagrama de solução.</t>
-  </si>
-  <si>
     <t>O site deverá ter uma calculadora financeira.</t>
   </si>
   <si>
@@ -191,21 +164,6 @@
     <t>O site institucional deverá ter um dark theme.</t>
   </si>
   <si>
-    <t>O software deverá ter tabelas criadas no MySQL (inserção de registros e consulta de dados).</t>
-  </si>
-  <si>
-    <t>O projeto deverá ter um protótipo do site institucional.</t>
-  </si>
-  <si>
-    <t>O software deverá ter uma documentação de justificativa de projeto.</t>
-  </si>
-  <si>
-    <t>O software deverá ter uma documentação de contexto de negócio.</t>
-  </si>
-  <si>
-    <t>O software deverá estar configurado no Github.</t>
-  </si>
-  <si>
     <t>Vinicius Novais</t>
   </si>
   <si>
@@ -222,6 +180,36 @@
   </si>
   <si>
     <t>O software deverá ter um simulador de Arduino (Execução de códigos e teste do sensor).</t>
+  </si>
+  <si>
+    <t>Nivelamento</t>
+  </si>
+  <si>
+    <t>O software deve permitir que a empresa gere relatorios atraves dos dados obtidos.</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma documentação de contexto de negócio e justificativa de projeto</t>
+  </si>
+  <si>
+    <t>O projeto deverá ter um site institucional.</t>
+  </si>
+  <si>
+    <t>O software deverá ter um banco de dados no MySQL (inserção de registros e consulta de dados).</t>
+  </si>
+  <si>
+    <t>O software deverá ter um HLD e LLD</t>
+  </si>
+  <si>
+    <t>Alessandro Raul</t>
+  </si>
+  <si>
+    <t>Caio Elcio</t>
+  </si>
+  <si>
+    <t>Luan Collyns</t>
+  </si>
+  <si>
+    <t>Luiz Gustavo</t>
   </si>
 </sst>
 </file>
@@ -254,7 +242,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,8 +297,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -387,17 +393,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -446,6 +459,22 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1168,10 +1197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G36"/>
+  <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1179,376 +1208,402 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="149.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="21"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+      <c r="E14" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="23">
+        <v>21</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="23">
+        <v>21</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+      <c r="D19" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="23">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="23">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
+      <c r="C21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="22">
+        <v>13</v>
+      </c>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="23">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="23">
+        <v>21</v>
+      </c>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="25">
         <v>3</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="19" t="s">
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E26" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="19" t="s">
+      <c r="F27" s="24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="8" t="s">
+      <c r="E29" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B16" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B25" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B27" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B31" s="12"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-    </row>
-    <row r="32" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B32" s="12"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="F29" s="23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="10"/>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B32" s="10"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B33" s="12"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C36" s="2"/>
+      <c r="C36" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1767,18 +1822,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1801,18 +1856,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A69715-2BF2-473E-A417-403290B48624}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6307CC5C-35AE-4BF6-AB1C-CA68C1295C47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A69715-2BF2-473E-A417-403290B48624}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
subindo mas foi o luan q fez
</commit_message>
<xml_diff>
--- a/Apresentação Sprint 2/Backlog.xlsx
+++ b/Apresentação Sprint 2/Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizg\Downloads\BandTec\Pesquisa e Inovação - Profº Brandão\Projeto PI - Sprint2\Projeto-PI\Apresentação Sprint 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F631B7-2739-4F58-A2F0-AC7A64EBB7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6FC1C1-10AA-49BF-900E-9900C5169C09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,9 +149,6 @@
     <t>RF18</t>
   </si>
   <si>
-    <t>O software deverá ter Wi-fi.</t>
-  </si>
-  <si>
     <t>O site deverá ter uma calculadora financeira.</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>Luiz Gustavo</t>
+  </si>
+  <si>
+    <t>O software deverá ter uma rede de dados.</t>
   </si>
 </sst>
 </file>
@@ -1200,7 +1200,7 @@
   <dimension ref="A2:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1218,12 +1218,12 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1233,17 +1233,17 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1264,7 +1264,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
@@ -1289,7 +1289,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>5</v>
@@ -1306,7 +1306,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>18</v>
@@ -1340,7 +1340,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>5</v>
@@ -1357,7 +1357,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>5</v>
@@ -1375,7 +1375,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>5</v>
@@ -1411,7 +1411,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>5</v>
@@ -1429,7 +1429,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>5</v>
@@ -1447,7 +1447,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>5</v>
@@ -1465,7 +1465,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>5</v>
@@ -1483,7 +1483,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>18</v>
@@ -1500,13 +1500,13 @@
         <v>26</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>13</v>
+      <c r="E25" s="14" t="s">
+        <v>6</v>
       </c>
       <c r="F25" s="22">
         <v>13</v>
@@ -1517,13 +1517,13 @@
         <v>27</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>13</v>
+      <c r="E26" s="14" t="s">
+        <v>6</v>
       </c>
       <c r="F26" s="23">
         <v>21</v>
@@ -1534,7 +1534,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>5</v>
@@ -1551,7 +1551,7 @@
         <v>29</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>18</v>
@@ -1568,7 +1568,7 @@
         <v>30</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>5</v>
@@ -1822,18 +1822,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1856,18 +1856,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A69715-2BF2-473E-A417-403290B48624}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6307CC5C-35AE-4BF6-AB1C-CA68C1295C47}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7A69715-2BF2-473E-A417-403290B48624}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>